<commit_message>
added user roles, permissions, check permission of users
</commit_message>
<xml_diff>
--- a/Database schemas.xlsx
+++ b/Database schemas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t xml:space="preserve">**User**</t>
   </si>
@@ -91,10 +91,16 @@
     <t xml:space="preserve">created_at</t>
   </si>
   <si>
+    <t xml:space="preserve">comment</t>
+  </si>
+  <si>
     <t xml:space="preserve">deadline</t>
   </si>
   <si>
     <t xml:space="preserve">project_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Project user**</t>
   </si>
 </sst>
 </file>
@@ -190,15 +196,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:I21"/>
+  <dimension ref="A4:I27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2551020408163"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8673469387755"/>
@@ -327,6 +334,9 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="C17" s="0" t="s">
         <v>19</v>
       </c>
@@ -344,6 +354,9 @@
       <c r="E18" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="G18" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
@@ -352,12 +365,32 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>